<commit_message>
update excel file and added some networkx tests
</commit_message>
<xml_diff>
--- a/lieux.xlsx
+++ b/lieux.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,23 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elève\Desktop\nf6_laposte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{78DE0030-7821-4E94-897F-C62E993C339A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E1D32B-7571-4E48-8855-E71F2DD53604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>capacité</t>
+  </si>
+  <si>
+    <t>recharge</t>
+  </si>
+  <si>
+    <t>autonomie</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,10 +379,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -468,4 +479,30 @@
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63AE29D-75C5-4804-A875-68A075B921E7}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix c algorithm and add functions to python
</commit_message>
<xml_diff>
--- a/lieux.xlsx
+++ b/lieux.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elève\Desktop\nf6_laposte\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alban\Desktop\Dev\laposte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E1D32B-7571-4E48-8855-E71F2DD53604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3CD435-8BB6-4336-86F3-AB996F8F2842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>capacité</t>
   </si>
@@ -30,6 +30,15 @@
   </si>
   <si>
     <t>autonomie</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>vitesse</t>
   </si>
 </sst>
 </file>
@@ -380,100 +389,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>-10</v>
+      </c>
+      <c r="B3">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>2</v>
       </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
+      <c r="B11">
         <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -483,15 +495,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63AE29D-75C5-4804-A875-68A075B921E7}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,6 +512,37 @@
       </c>
       <c r="C1" t="s">
         <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>80</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add c docs (in code comments)
</commit_message>
<xml_diff>
--- a/lieux.xlsx
+++ b/lieux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alban\Desktop\Dev\laposte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3CD435-8BB6-4336-86F3-AB996F8F2842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CF9083-B3AC-4A05-A00E-17AD55A52656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,6 +488,70 @@
         <v>6</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>-6</v>
+      </c>
+      <c r="B12">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>-7</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>-3</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>-2</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
 </worksheet>
@@ -497,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63AE29D-75C5-4804-A875-68A075B921E7}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,13 +583,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="D2">
         <v>50</v>
@@ -533,13 +597,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="D3">
         <v>50</v>

</xml_diff>